<commit_message>
Debug all scripts under smoke test folder.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/400.20.10_ApplicationNformToolsServiceControl.xlsx
+++ b/NformTester/NformTester/Keywordscripts/400.20.10_ApplicationNformToolsServiceControl.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="270" yWindow="2535" windowWidth="15480" windowHeight="11640"/>
@@ -1200,7 +1200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7372" uniqueCount="827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7372" uniqueCount="828">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -3740,6 +3740,10 @@
   <si>
     <t xml:space="preserve">;Clear configuration </t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4683,7 +4687,7 @@
   <dimension ref="A1:O104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4813,7 +4817,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>796</v>
+        <v>827</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>191</v>
@@ -6497,7 +6501,7 @@
         <v>63</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>796</v>
+        <v>827</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>191</v>

</xml_diff>